<commit_message>
conversão de nome para siglas
</commit_message>
<xml_diff>
--- a/Data/g1.1.xlsx
+++ b/Data/g1.1.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Roraima</t>
+          <t>RR</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -479,7 +479,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Roraima</t>
+          <t>RR</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -492,7 +492,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mato Grosso</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -503,7 +503,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Mato Grosso</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -516,7 +516,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Piauí</t>
+          <t>PI</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -527,7 +527,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Tocantins</t>
+          <t>TO</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -540,7 +540,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tocantins</t>
+          <t>TO</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -551,7 +551,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Piauí</t>
+          <t>PI</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -564,7 +564,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Acre</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -575,7 +575,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Mato Grosso do Sul</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -588,7 +588,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Paraíba</t>
+          <t>PB</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -599,7 +599,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Maranhão</t>
+          <t>MA</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -612,7 +612,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>SE</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -623,7 +623,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>SE</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -636,7 +636,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -645,7 +645,7 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -656,7 +656,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -665,7 +665,7 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E10" t="n">

</xml_diff>

<commit_message>
g1.1 e g1.3 - reestruturação do arquivo
</commit_message>
<xml_diff>
--- a/Data/g1.1.xlsx
+++ b/Data/g1.1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -451,17 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>UF</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Variação (%) 2022/2010</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Rank</t>
+          <t>Categoria</t>
         </is>
       </c>
     </row>
@@ -479,14 +469,8 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>RR</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>57.303631404687</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
+          <t>Variação (%) 2022</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -503,14 +487,8 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>MT</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>56.93075937581798</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2</v>
+          <t>Variação (%) 2022</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -527,14 +505,8 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TO</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>47.69781593734575</v>
-      </c>
-      <c r="F4" t="n">
-        <v>3</v>
+          <t>Variação (%) 2022</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -551,14 +523,8 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PI</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>32.6068937425523</v>
-      </c>
-      <c r="F5" t="n">
-        <v>4</v>
+          <t>Variação (%) 2022</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -575,14 +541,8 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>MS</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>31.84788151928765</v>
-      </c>
-      <c r="F6" t="n">
-        <v>5</v>
+          <t>Variação (%) 2022</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -599,14 +559,8 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>MA</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>29.69759694720014</v>
-      </c>
-      <c r="F7" t="n">
-        <v>6</v>
+          <t>Variação (%) 2022</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -623,14 +577,8 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SE</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>4.078908858016646</v>
-      </c>
-      <c r="F8" t="n">
-        <v>26</v>
+          <t>Variação (%) 2022</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -645,13 +593,9 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>BR</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>11.52892348592597</v>
-      </c>
-      <c r="F9" t="inlineStr"/>
+          <t>Variação (%) 2022</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -665,13 +609,167 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
+          <t>Variação (%) 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>RR</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>57.303631404687</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Variação (%) 2022/2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>56.93075937581798</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Variação (%) 2022/2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>47.69781593734575</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Variação (%) 2022/2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>PI</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>32.6068937425523</v>
+      </c>
+      <c r="C14" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Variação (%) 2022/2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>31.84788151928765</v>
+      </c>
+      <c r="C15" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Variação (%) 2022/2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>29.69759694720014</v>
+      </c>
+      <c r="C16" t="n">
+        <v>6</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Variação (%) 2022/2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4.078908858016646</v>
+      </c>
+      <c r="C17" t="n">
+        <v>26</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Variação (%) 2022/2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>11.52892348592597</v>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Variação (%) 2022/2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>NE</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="B19" t="n">
         <v>13.60673175406315</v>
       </c>
-      <c r="F10" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Variação (%) 2022/2010</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Script 1 - atualização automática de dados
</commit_message>
<xml_diff>
--- a/Data/g1.1.xlsx
+++ b/Data/g1.1.xlsx
@@ -458,54 +458,54 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11.28257356816728</v>
+        <v>14.73257689442189</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.38328592034125</v>
+        <v>13.44269577606423</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PI</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.163532889959003</v>
+        <v>12.88001598426398</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
@@ -516,50 +516,50 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6.038578912774967</v>
+        <v>7.890383025089162</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5.979340654464274</v>
+        <v>5.652659822157795</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PB</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5.639044878530812</v>
+        <v>4.816953216278661</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
@@ -570,14 +570,14 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.251393607016045</v>
+        <v>3.118144130554446</v>
       </c>
       <c r="C8" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
@@ -588,12 +588,12 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3.016694345902016</v>
+        <v>3.241657824791806</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
@@ -604,48 +604,48 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3.554673531071183</v>
+        <v>2.867008788862638</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>57.303631404687</v>
+        <v>77.14346626765018</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>RR</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>56.93075937581798</v>
+        <v>63.84407511155798</v>
       </c>
       <c r="C12" t="n">
         <v>2</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
@@ -656,68 +656,68 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>47.69781593734575</v>
+        <v>59.35173933449352</v>
       </c>
       <c r="C13" t="n">
         <v>3</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PI</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>32.6068937425523</v>
+        <v>49.57179111911111</v>
       </c>
       <c r="C14" t="n">
         <v>4</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>31.84788151928765</v>
+        <v>42.69524774665621</v>
       </c>
       <c r="C15" t="n">
         <v>5</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MA</t>
+          <t>PI</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>29.69759694720014</v>
+        <v>36.70681689547283</v>
       </c>
       <c r="C16" t="n">
         <v>6</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
@@ -728,14 +728,14 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>4.078908858016646</v>
+        <v>7.324239245718005</v>
       </c>
       <c r="C17" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
@@ -746,12 +746,12 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>11.52892348592597</v>
+        <v>15.14430956101356</v>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
@@ -762,12 +762,12 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>13.60673175406315</v>
+        <v>16.86384673819174</v>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Script 1 - atualização automática de dados (Execução: 22)
</commit_message>
<xml_diff>
--- a/Data/g1.1.xlsx
+++ b/Data/g1.1.xlsx
@@ -458,54 +458,54 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11.28257356816728</v>
+        <v>14.73257689442189</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.38328592034125</v>
+        <v>13.44269577606423</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PI</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.163532889959003</v>
+        <v>12.88001598426398</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
@@ -516,50 +516,50 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6.038578912774967</v>
+        <v>7.890383025089162</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5.979340654464274</v>
+        <v>5.652659822157795</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PB</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5.639044878530812</v>
+        <v>4.816953216278661</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
@@ -570,14 +570,14 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.251393607016045</v>
+        <v>3.118144130554446</v>
       </c>
       <c r="C8" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
@@ -588,12 +588,12 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3.016694345902016</v>
+        <v>3.241657824791806</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
@@ -604,48 +604,48 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3.554673531071183</v>
+        <v>2.867008788862638</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>57.303631404687</v>
+        <v>77.14346626765018</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>RR</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>56.93075937581798</v>
+        <v>63.84407511155798</v>
       </c>
       <c r="C12" t="n">
         <v>2</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
@@ -656,68 +656,68 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>47.69781593734575</v>
+        <v>59.35173933449352</v>
       </c>
       <c r="C13" t="n">
         <v>3</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PI</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>32.6068937425523</v>
+        <v>49.57179111911111</v>
       </c>
       <c r="C14" t="n">
         <v>4</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>31.84788151928765</v>
+        <v>42.69524774665621</v>
       </c>
       <c r="C15" t="n">
         <v>5</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MA</t>
+          <t>PI</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>29.69759694720014</v>
+        <v>36.70681689547283</v>
       </c>
       <c r="C16" t="n">
         <v>6</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
@@ -728,14 +728,14 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>4.078908858016646</v>
+        <v>7.324239245718005</v>
       </c>
       <c r="C17" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
@@ -746,12 +746,12 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>11.52892348592597</v>
+        <v>15.14430956101356</v>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
@@ -762,12 +762,12 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>13.60673175406315</v>
+        <v>16.86384673819174</v>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Script 1 - atualização automática de dados (Execução: 23)
</commit_message>
<xml_diff>
--- a/Data/g1.1.xlsx
+++ b/Data/g1.1.xlsx
@@ -458,54 +458,54 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11.28257356816728</v>
+        <v>14.73257689442189</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.38328592034125</v>
+        <v>13.44269577606423</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PI</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.163532889959003</v>
+        <v>12.88001598426398</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
@@ -516,50 +516,50 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6.038578912774967</v>
+        <v>7.890383025089162</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5.979340654464274</v>
+        <v>5.652659822157795</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PB</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5.639044878530812</v>
+        <v>4.816953216278661</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
@@ -570,14 +570,14 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.251393607016045</v>
+        <v>3.118144130554446</v>
       </c>
       <c r="C8" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
@@ -588,12 +588,12 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3.016694345902016</v>
+        <v>3.241657824791806</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
@@ -604,48 +604,48 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3.554673531071183</v>
+        <v>2.867008788862638</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Variação (%) 2022</t>
+          <t>Variação (%) 2023</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>57.303631404687</v>
+        <v>77.14346626765018</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>RR</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>56.93075937581798</v>
+        <v>63.84407511155798</v>
       </c>
       <c r="C12" t="n">
         <v>2</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
@@ -656,68 +656,68 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>47.69781593734575</v>
+        <v>59.35173933449352</v>
       </c>
       <c r="C13" t="n">
         <v>3</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PI</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>32.6068937425523</v>
+        <v>49.57179111911111</v>
       </c>
       <c r="C14" t="n">
         <v>4</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>31.84788151928765</v>
+        <v>42.69524774665621</v>
       </c>
       <c r="C15" t="n">
         <v>5</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MA</t>
+          <t>PI</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>29.69759694720014</v>
+        <v>36.70681689547283</v>
       </c>
       <c r="C16" t="n">
         <v>6</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
@@ -728,14 +728,14 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>4.078908858016646</v>
+        <v>7.324239245718005</v>
       </c>
       <c r="C17" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
@@ -746,12 +746,12 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>11.52892348592597</v>
+        <v>15.14430956101356</v>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>
@@ -762,12 +762,12 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>13.60673175406315</v>
+        <v>16.86384673819174</v>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Variação (%) 2022/2010</t>
+          <t>Variação (%) 2023/2010</t>
         </is>
       </c>
     </row>

</xml_diff>